<commit_message>
instruction table no excel
</commit_message>
<xml_diff>
--- a/09 - Week 7/QR.xlsx
+++ b/09 - Week 7/QR.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A24497-D641-47DE-9784-63F024F092C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A913A0-B242-4A10-AEAA-78F5244712FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR Codes" sheetId="1" r:id="rId1"/>
     <sheet name="Assembly" sheetId="3" r:id="rId2"/>
+    <sheet name="Instruction" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="39">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -111,6 +112,55 @@
   </si>
   <si>
     <t>Pieces Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Instruction Data</t>
+  </si>
+  <si>
+    <t>ID da Instrução</t>
+  </si>
+  <si>
+    <t>Passo 1</t>
+  </si>
+  <si>
+    <t>Passo 2</t>
+  </si>
+  <si>
+    <t>Passo 3</t>
+  </si>
+  <si>
+    <t>Passo 4</t>
+  </si>
+  <si>
+    <t>Exemplo</t>
+  </si>
+  <si>
+    <t>3011
+#f0e1ff
+2
+0
+4</t>
+  </si>
+  <si>
+    <t>3437
+#f0e100
+5
+1
+2</t>
+  </si>
+  <si>
+    <t>3437
+#f0e1f0
+2
+2
+5</t>
+  </si>
+  <si>
+    <t>3011
+#f0ef50
+2
+0
+4</t>
   </si>
 </sst>
 </file>
@@ -777,7 +827,7 @@
     <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -855,6 +905,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Cor1" xfId="24" builtinId="30" customBuiltin="1"/>
@@ -905,7 +958,69 @@
     <cellStyle name="Verificar Célula" xfId="18" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="74">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -923,57 +1038,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
         <top style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14993743705557422"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -994,18 +1078,54 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0" tint="-4.9989318521683403E-2"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
+        <left/>
         <right style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </right>
@@ -1014,43 +1134,6 @@
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14993743705557422"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -1071,55 +1154,15 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14993743705557422"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
+        <left/>
         <right style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </right>
@@ -1129,6 +1172,8 @@
         <bottom style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1325,8 +1370,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -1344,7 +1387,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
@@ -1355,8 +1398,6 @@
         <bottom style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1397,121 +1438,25 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14993743705557422"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color rgb="FFD9D9D9"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFD9D9D9"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -1547,14 +1492,6 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1578,13 +1515,6 @@
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color rgb="FFD9D9D9"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1616,16 +1546,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -2231,8 +2151,148 @@
     <dxf>
       <border>
         <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color rgb="FFD9D9D9"/>
         </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF595959"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFF2F2F2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color rgb="FFD9D9D9"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFD9D9D9"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF595959"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color rgb="FFD9D9D9"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2253,26 +2313,60 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
         <right style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -2296,6 +2390,543 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="34" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
       <alignment vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2339,16 +2970,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -2414,13 +3035,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CollegeBudget2" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="54"/>
-      <tableStyleElement type="headerRow" dxfId="53"/>
-      <tableStyleElement type="totalRow" dxfId="52"/>
-      <tableStyleElement type="firstColumn" dxfId="51"/>
-      <tableStyleElement type="lastColumn" dxfId="50"/>
-      <tableStyleElement type="firstRowStripe" dxfId="49"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="73"/>
+      <tableStyleElement type="headerRow" dxfId="72"/>
+      <tableStyleElement type="totalRow" dxfId="71"/>
+      <tableStyleElement type="firstColumn" dxfId="70"/>
+      <tableStyleElement type="lastColumn" dxfId="69"/>
+      <tableStyleElement type="firstRowStripe" dxfId="68"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="67"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -3281,33 +3902,359 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>12701</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F93C83D8-AACA-4053-967D-14A917BE8E8E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="15826" t="14479" r="17172" b="21887"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="660400" y="264161"/>
+          <a:ext cx="1046480" cy="1191259"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="333333">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{406B9709-85C8-4573-8724-004B9203B262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="13335000" y="6134100"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1463039</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F528905-3445-7170-D5AC-4784DE779EE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1348740" y="4488180"/>
+          <a:ext cx="1463039" cy="1645920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>266701</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1422</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1645920</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>15241</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B09BA6C9-A216-6C52-C142-0C1CF233BD02}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3086101" y="4489602"/>
+          <a:ext cx="1379219" cy="1659739"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>198122</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1643159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1600200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>7621</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagem 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5EFC5B8-E9DB-114D-E45F-1C15946906B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4846322" y="4485419"/>
+          <a:ext cx="1402078" cy="1656302"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>403861</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1790700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1635759</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagem 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC7070B-AF95-581E-45C0-01F393D365AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6774181" y="4488180"/>
+          <a:ext cx="1386839" cy="1635759"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:I17" totalsRowShown="0" headerRowDxfId="45" dataDxfId="43" totalsRowDxfId="41" headerRowBorderDxfId="44" tableBorderDxfId="42" totalsRowBorderDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:I17" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" totalsRowDxfId="62" headerRowBorderDxfId="65" tableBorderDxfId="63" totalsRowBorderDxfId="61">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Identificador da Peça (ID) " dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{3341B563-EB1E-48B1-94F1-39D1CCC81DB5}" name="Color" dataDxfId="37" totalsRowDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{8AA3327B-937D-49A5-B348-71770C55EC1E}" name="X" dataDxfId="35" totalsRowDxfId="34"/>
-    <tableColumn id="7" xr3:uid="{DC76DAEF-1023-465D-B5B8-87789D86CF69}" name="Y" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{E5EA106A-A2AC-4D91-A44D-43F37D0C4A85}" name="Z" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Identificador da Peça (ID) " dataDxfId="60" totalsRowDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{3341B563-EB1E-48B1-94F1-39D1CCC81DB5}" name="Color" dataDxfId="58" totalsRowDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{8AA3327B-937D-49A5-B348-71770C55EC1E}" name="X" dataDxfId="56" totalsRowDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{DC76DAEF-1023-465D-B5B8-87789D86CF69}" name="Y" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{E5EA106A-A2AC-4D91-A44D-43F37D0C4A85}" name="Z" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="46" totalsRowDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A20313AD-BF3F-491B-8443-B62911D01060}" name="Table_AcademicExpenses6" displayName="Table_AcademicExpenses6" ref="B7:I17" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" totalsRowDxfId="17" headerRowBorderDxfId="20" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A20313AD-BF3F-491B-8443-B62911D01060}" name="Table_AcademicExpenses6" displayName="Table_AcademicExpenses6" ref="B7:I17" totalsRowShown="0" headerRowDxfId="44" dataDxfId="42" totalsRowDxfId="40" headerRowBorderDxfId="43" tableBorderDxfId="41" totalsRowBorderDxfId="39">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BB7F2196-2B5F-48C4-9448-0E4DC098762A}" name="Identificador da Montagem  (ID) " dataDxfId="15" totalsRowDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{1C894641-CB47-4458-8D3E-83821726DF13}" name="Peça 1" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{AC6DB513-F3D7-494B-89B0-800144100474}" name="Peça 2" dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{5A7909B8-B36B-4D1E-BB35-511363441A82}" name="Peça 3" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{22F8AD07-1F90-4CA5-A0F5-4DA4BFC326EA}" name="Peça 4" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{04291E92-9D35-42F7-ABEE-9343325C1F32}" name="Nome" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{EFA8F15D-584F-4C04-945A-3DED2B8B5624}" name="Montagem" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7650E1EE-5811-48C9-8355-23A998B379C7}" name="QR Code" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{BB7F2196-2B5F-48C4-9448-0E4DC098762A}" name="Identificador da Montagem  (ID) " dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{1C894641-CB47-4458-8D3E-83821726DF13}" name="Peça 1" dataDxfId="36" totalsRowDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{AC6DB513-F3D7-494B-89B0-800144100474}" name="Peça 2" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{5A7909B8-B36B-4D1E-BB35-511363441A82}" name="Peça 3" dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{22F8AD07-1F90-4CA5-A0F5-4DA4BFC326EA}" name="Peça 4" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{04291E92-9D35-42F7-ABEE-9343325C1F32}" name="Nome" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{EFA8F15D-584F-4C04-945A-3DED2B8B5624}" name="Montagem" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{7650E1EE-5811-48C9-8355-23A998B379C7}" name="QR Code" dataDxfId="24" totalsRowDxfId="23"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAEE89A6-4045-46DA-8B0A-A8F7614937A7}" name="Table_AcademicExpenses64" displayName="Table_AcademicExpenses64" ref="B7:G17" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{74E7D2D3-B442-4085-A649-9E14A2E1EED8}" name="ID da Instrução" dataDxfId="15" totalsRowDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{2B96773D-1149-4682-8095-004001D28840}" name="Passo 1" dataDxfId="13" totalsRowDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{5CBFF619-747B-4399-8F8B-3B3FF811D706}" name="Passo 2" dataDxfId="11" totalsRowDxfId="12"/>
+    <tableColumn id="7" xr3:uid="{D695FA95-21D4-4BB9-8F20-81669AB91971}" name="Passo 3" dataDxfId="9" totalsRowDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{EA9968B6-4B3E-4436-8437-EF6A13BD059D}" name="Passo 4" dataDxfId="7" totalsRowDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{BF12C0E8-435E-421B-A167-61166A62AB84}" name="Nome" dataDxfId="5" totalsRowDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3578,27 +4525,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.90625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.453125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.26953125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="1.7265625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="1" width="1.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.44140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.21875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="40.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="1.77734375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
         <v>27</v>
       </c>
@@ -3610,35 +4557,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:17" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="2:17" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" s="10" customFormat="1" ht="36.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:17" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
         <v>6</v>
       </c>
@@ -3664,7 +4611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>3437</v>
       </c>
@@ -3685,7 +4632,7 @@
       <c r="I8" s="8"/>
       <c r="N8" s="16"/>
     </row>
-    <row r="9" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>3011</v>
       </c>
@@ -3709,7 +4656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>76371</v>
       </c>
@@ -3731,7 +4678,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -3741,7 +4688,7 @@
       <c r="H11"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="2:17" s="10" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" s="10" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -3751,7 +4698,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="2:17" s="3" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" s="3" customFormat="1" ht="128.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -3761,7 +4708,7 @@
       <c r="H13"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -3774,7 +4721,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:17" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" ht="129.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -3785,7 +4732,7 @@
       <c r="I15" s="8"/>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -3795,7 +4742,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="2:9" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -3805,80 +4752,80 @@
       <c r="H17" s="15"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:9" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" s="10" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
     </row>
-    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B31:F31"/>
@@ -3901,12 +4848,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="expression" dxfId="47" priority="1">
+    <cfRule type="expression" dxfId="4" priority="1">
       <formula>H14&gt;G14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:E5">
-    <cfRule type="expression" dxfId="46" priority="6">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3957,27 +4904,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF356DD-DB4F-4976-BB2F-7A7B3D324CA4}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection sqref="A1:XFD17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.90625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="24" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.08984375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.6328125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.08984375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="40.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" style="1" customWidth="1"/>
-    <col min="10" max="11" width="1.7265625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.1796875" style="1"/>
+    <col min="8" max="8" width="40.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="25.77734375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="1.77734375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:17" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:17" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:17" customFormat="1" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
         <v>15</v>
       </c>
@@ -3989,35 +4936,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:17" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:17" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="2:17" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:17" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="2:17" s="10" customFormat="1" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:17" s="10" customFormat="1" ht="36.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="2:17" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:17" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="21"/>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:17" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="22" t="s">
         <v>16</v>
       </c>
@@ -4043,7 +4990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18">
         <v>12345</v>
       </c>
@@ -4066,7 +5013,7 @@
       <c r="I8" s="8"/>
       <c r="N8" s="16"/>
     </row>
-    <row r="9" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="18">
         <v>23456</v>
       </c>
@@ -4091,7 +5038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="18">
         <v>34567</v>
       </c>
@@ -4113,7 +5060,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:17" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="7"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
@@ -4123,7 +5070,7 @@
       <c r="H11"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="2:17" s="10" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:17" s="10" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="7"/>
       <c r="C12" s="18"/>
       <c r="D12" s="18"/>
@@ -4133,7 +5080,7 @@
       <c r="H12" s="20"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="2:17" s="3" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:17" s="3" customFormat="1" ht="128.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7"/>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -4143,7 +5090,7 @@
       <c r="H13"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -4153,7 +5100,7 @@
       <c r="H14" s="15"/>
       <c r="I14" s="8"/>
     </row>
-    <row r="15" spans="2:17" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:17" ht="129.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -4164,7 +5111,7 @@
       <c r="I15" s="8"/>
       <c r="Q15" s="16"/>
     </row>
-    <row r="16" spans="2:17" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:17" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -4174,7 +5121,7 @@
       <c r="H16" s="15"/>
       <c r="I16" s="8"/>
     </row>
-    <row r="17" spans="2:9" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:9" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -4184,80 +5131,80 @@
       <c r="H17" s="15"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
       <c r="D19" s="26"/>
       <c r="E19" s="26"/>
       <c r="F19" s="26"/>
     </row>
-    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
     </row>
-    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
     </row>
-    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:9" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:9" s="10" customFormat="1" ht="37.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
     </row>
-    <row r="25" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:9" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:9" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
     </row>
-    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
     </row>
-    <row r="28" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
     </row>
-    <row r="29" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
     </row>
-    <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B31" s="23"/>
       <c r="C31" s="23"/>
       <c r="D31" s="23"/>
       <c r="E31" s="23"/>
       <c r="F31" s="23"/>
     </row>
-    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="33" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:F2"/>
@@ -4279,12 +5226,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>H14&gt;G14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:E5">
-    <cfRule type="expression" dxfId="22" priority="3">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4331,7 +5278,278 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1C7DB9-6A79-4D22-A558-4FB1BAC48714}">
+  <dimension ref="B1:O17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" customWidth="1"/>
+    <col min="7" max="7" width="34.77734375" customWidth="1"/>
+    <col min="8" max="8" width="46.5546875" customWidth="1"/>
+    <col min="9" max="9" width="133" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" s="1" customFormat="1" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="2:15" ht="94.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" spans="2:15" s="1" customFormat="1" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="2:15" s="10" customFormat="1" ht="36.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="2:15" s="3" customFormat="1" ht="37.5" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="21"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="2:15" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" s="1" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="18">
+        <v>50999</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="2:15" s="1" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="18"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="15"/>
+      <c r="L9" s="16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="2:15" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="15"/>
+    </row>
+    <row r="12" spans="2:15" s="10" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="7"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="2:15" s="3" customFormat="1" ht="128.55000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="7"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="2:15" s="1" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="2:15" s="1" customFormat="1" ht="129.44999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="15"/>
+      <c r="O15" s="16"/>
+    </row>
+    <row r="16" spans="2:15" s="1" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="15"/>
+    </row>
+    <row r="17" spans="2:7" s="1" customFormat="1" ht="130.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="0">
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="4" tint="-0.249977111117893"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BE556F88-A637-488B-88FA-A6A58DA961D9}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:E5">
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>#REF!&gt;#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations xWindow="152" yWindow="518" count="6">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Orçamento Universitário Mensal" prompt="Este modelo monitoriza as suas despesas reais em relação ao seu orçamento universitário mensal._x000a__x000a_Introduzia os seus itens de despesa e orçamento nas três tabelas. Atualize a coluna Gastos Reais à medida que gasta dinheiro._x000a_" sqref="A2" xr:uid="{BF6A4BF5-4888-41BE-9587-43F69BD37B1B}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza o Orçamento por item sob esta coluna" sqref="G7" xr:uid="{56D4513E-B7F9-4382-8EDF-C2F9F8508581}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O Orçamento Total Mensal é calculado nesta célula" sqref="B5" xr:uid="{A6692070-00AD-47AE-9855-6D70D715BD8C}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O total dos gastos reais é calculado nesta célula" sqref="C5:E5" xr:uid="{19DD37B3-A111-4D50-94F9-A3B0FE5A0A5F}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta barra mostra a % do dinheiro gasto em relação ao orçamento total" sqref="F5" xr:uid="{7F36BFB5-04CF-4AB3-B24D-36331ACD7DDE}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza Itens de Despesa abaixo desta coluna" sqref="B7:F7" xr:uid="{70BFDB82-3648-403F-A42F-587B8683634B}"/>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BE556F88-A637-488B-88FA-A6A58DA961D9}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -4619,36 +5837,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03FCA663-A0D5-4D37-87D6-2910454B74A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D95769C4-607B-4664-9C36-EC9F8E41992B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FE855E-B5B1-4D66-876A-F04E3BDA8A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4667,24 +5876,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D95769C4-607B-4664-9C36-EC9F8E41992B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03FCA663-A0D5-4D37-87D6-2910454B74A5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
catalogo & new assemblies
</commit_message>
<xml_diff>
--- a/09 - Week 7/QR.xlsx
+++ b/09 - Week 7/QR.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8314FEA0-7C95-445B-BF4A-84C7BF7AC135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6534C7AB-94F5-417A-811A-A0B54D53CC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="469" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" tabRatio="469" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QR Codes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="57">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -88,15 +88,6 @@
   </si>
   <si>
     <t>Montagem</t>
-  </si>
-  <si>
-    <t> 76371</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Bricks</t>
   </si>
   <si>
     <t>Pieces Data</t>
@@ -183,8 +174,65 @@
 coordinates: {x:4, y:2}</t>
   </si>
   <si>
+    <t>flower</t>
+  </si>
+  <si>
     <t>idPiece: 3011W
-idStep: 12345D
+idStep: a23456
+color:white
+coordinates: {x:6, y:1}</t>
+  </si>
+  <si>
+    <t>idPiece: 3011Y
+idStep: b23456
+color: yellow
+coordinates: {x:6, y:5}</t>
+  </si>
+  <si>
+    <t>idPiece: 3437O
+idStep: c23456
+color: orange
+coordinates: {x:4, y:3}</t>
+  </si>
+  <si>
+    <t>idPiece: 3011W
+idStep: d12345
+color: white
+coordinates: {x:6, y:2}</t>
+  </si>
+  <si>
+    <t>idPiece: 3437B
+idStep: d23456
+color: blue
+coordinates: {x:10, y:3}</t>
+  </si>
+  <si>
+    <t> 76371R</t>
+  </si>
+  <si>
+    <t>strips</t>
+  </si>
+  <si>
+    <t>idPiece: 76371R
+idStep: a34567
+color:red
+coordinates: {x:10, y:2}</t>
+  </si>
+  <si>
+    <t>idPiece: 76371R
+idStep: b34567
+color: red
+coordinates: {x:10, y:4}</t>
+  </si>
+  <si>
+    <t>idPiece: 3011Y
+idStep: c34567
+color: yellow
+coordinates: {x:6, y:2}</t>
+  </si>
+  <si>
+    <t>idPiece: 3011W
+idStep: d34567
 color: white
 coordinates: {x:6, y:2}</t>
   </si>
@@ -200,7 +248,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="#,##0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -435,6 +483,23 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1" tint="0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -853,7 +918,7 @@
     <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -925,6 +990,12 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="9"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -990,31 +1061,6 @@
   <dxfs count="70">
     <dxf>
       <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1501,6 +1547,11 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2212,6 +2263,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -2846,6 +2907,16 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor theme="4" tint="0.79998168889431442"/>
@@ -2933,79 +3004,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1314450</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Logo">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E18D2F-9C85-7E12-D724-50803B979EA5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect l="15826" t="14479" r="17172" b="21887"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="146050" y="266700"/>
-          <a:ext cx="1263650" cy="1203325"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="76200" dist="38100" dir="7800000" algn="tl" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="40000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:scene3d>
-          <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="contrasting" dir="t">
-            <a:rot lat="0" lon="0" rev="4200000"/>
-          </a:lightRig>
-        </a:scene3d>
-        <a:sp3d prstMaterial="plastic">
-          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
-          <a:contourClr>
-            <a:srgbClr val="969696"/>
-          </a:contourClr>
-        </a:sp3d>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -3081,7 +3079,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3125,7 +3123,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3169,7 +3167,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3213,7 +3211,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3257,7 +3255,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3301,7 +3299,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3345,7 +3343,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3389,7 +3387,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3433,7 +3431,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3477,7 +3475,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3521,7 +3519,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3565,7 +3563,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3578,6 +3576,65 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1282700</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>1152111</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Logo">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0FD9823-24A0-4E25-A782-6DA6B576CC58}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="15826" t="14479" r="17172" b="21887"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="120650" y="196850"/>
+          <a:ext cx="1266825" cy="1212436"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="292100" dist="139700" dir="2700000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="333333">
+              <a:alpha val="65000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -3598,7 +3655,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>1314450</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>6350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3697,15 +3754,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>29417</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>19579</xdr:rowOff>
+      <xdr:colOff>4569</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>599362</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>85587</xdr:colOff>
+      <xdr:colOff>63914</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>84383</xdr:rowOff>
+      <xdr:rowOff>48078</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3734,8 +3791,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10804573" y="2867157"/>
-          <a:ext cx="2864061" cy="1711835"/>
+          <a:off x="10780243" y="2843949"/>
+          <a:ext cx="2870324" cy="1713043"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3755,7 +3812,7 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>1597422</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>1607770</xdr:rowOff>
+      <xdr:rowOff>1610945</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3779,6 +3836,193 @@
         <a:xfrm>
           <a:off x="13725128" y="2953544"/>
           <a:ext cx="1455341" cy="1501804"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1587500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>89297</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>226328</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1600597</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50A6BBAC-45D2-6BC5-2A7F-F7C81E61F313}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10685859" y="4583906"/>
+          <a:ext cx="3123516" cy="1511300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>39688</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>29766</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1745813</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1607345</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30D8D168-E7F4-BAA7-D68D-7EB86CCD148E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13622735" y="4524375"/>
+          <a:ext cx="1702950" cy="1574404"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>253587</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57807</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1675021</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1629315</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{736A8D90-9EBE-30C0-2C86-9E5D4E58AA63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:srcRect l="10894" r="8624" b="5310"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13837065" y="6211785"/>
+          <a:ext cx="1421434" cy="1571508"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>17935</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1565413</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63C62A34-71CC-EC6E-1512-59D5B7A0B5A2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10775674" y="6153978"/>
+          <a:ext cx="2825739" cy="1565413"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3862,7 +4106,7 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>134620</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -4099,48 +4343,491 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1266826</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1533526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>17003</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1616076</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E53BBB83-88DA-B23C-90A5-62EB8238323A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2638426" y="4391026"/>
+          <a:ext cx="2941177" cy="1730375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1390651</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>46735</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1381126</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04D624DA-08DC-2375-684B-7129CA6E484D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6953251" y="4581526"/>
+          <a:ext cx="2599434" cy="1304925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1212849</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1638300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>209781</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1554197</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagem 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{768E3FB1-05B7-E045-EFB3-83C76DD041CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10718799" y="4495800"/>
+          <a:ext cx="3168882" cy="1563722"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1625600</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>158963</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1620827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagem 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FEEA5989-E019-EEEE-523A-CE0FD7E8987F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15303500" y="4505326"/>
+          <a:ext cx="2810088" cy="1620826"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="1782445"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C47BEA3-1B80-4DFE-BB87-2F61088343B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="17954625" y="4505325"/>
+          <a:ext cx="304800" cy="1782445"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1390650</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>4184500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1530350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagem 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{484CD0C3-0B6F-EE27-9F07-8EC386837A8D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762250" y="6238875"/>
+          <a:ext cx="2793850" cy="1444625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152402</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1447630</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagem 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61362357-CBF3-096A-3B10-D05866110293}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896100" y="6305552"/>
+          <a:ext cx="2625725" cy="1295228"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1543050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161926</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>4150323</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1533526</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Imagem 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F3A48E-55D0-7745-693B-342482659864}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11049000" y="6315076"/>
+          <a:ext cx="2607273" cy="1371600"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>447920</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1572250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagem 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB8BF42A-8911-6889-7DE7-9672F81AFE08}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15049500" y="6248400"/>
+          <a:ext cx="3353045" cy="1477000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:H20" totalsRowShown="0" headerRowDxfId="62" dataDxfId="60" totalsRowDxfId="58" headerRowBorderDxfId="61" tableBorderDxfId="59" totalsRowBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:H20" totalsRowShown="0" headerRowDxfId="60" dataDxfId="58" totalsRowDxfId="56" headerRowBorderDxfId="59" tableBorderDxfId="57" totalsRowBorderDxfId="55">
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Identificador da Peça (ID) " dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="6" xr3:uid="{3341B563-EB1E-48B1-94F1-39D1CCC81DB5}" name="Color" dataDxfId="54" totalsRowDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{8AA3327B-937D-49A5-B348-71770C55EC1E}" name="X" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{E5EA106A-A2AC-4D91-A44D-43F37D0C4A85}" name="Y" dataDxfId="50" totalsRowDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="48" totalsRowDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="46" totalsRowDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Identificador da Peça (ID) " dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{3341B563-EB1E-48B1-94F1-39D1CCC81DB5}" name="Color" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="8" xr3:uid="{8AA3327B-937D-49A5-B348-71770C55EC1E}" name="X" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{E5EA106A-A2AC-4D91-A44D-43F37D0C4A85}" name="Y" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="42" totalsRowDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A20313AD-BF3F-491B-8443-B62911D01060}" name="Table_AcademicExpenses6" displayName="Table_AcademicExpenses6" ref="B7:I17" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" totalsRowDxfId="38" headerRowBorderDxfId="41" tableBorderDxfId="39" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A20313AD-BF3F-491B-8443-B62911D01060}" name="Table_AcademicExpenses6" displayName="Table_AcademicExpenses6" ref="B7:I17" totalsRowShown="0" headerRowDxfId="38" dataDxfId="36" totalsRowDxfId="34" headerRowBorderDxfId="37" tableBorderDxfId="35" totalsRowBorderDxfId="33">
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{BB7F2196-2B5F-48C4-9448-0E4DC098762A}" name="Identificador da Montagem  (ID) " dataDxfId="36" totalsRowDxfId="35"/>
-    <tableColumn id="6" xr3:uid="{1C894641-CB47-4458-8D3E-83821726DF13}" name="Peça 1" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="8" xr3:uid="{AC6DB513-F3D7-494B-89B0-800144100474}" name="Peça 2" dataDxfId="32" totalsRowDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{5A7909B8-B36B-4D1E-BB35-511363441A82}" name="Peça 3" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{22F8AD07-1F90-4CA5-A0F5-4DA4BFC326EA}" name="Peça 4" dataDxfId="28" totalsRowDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{04291E92-9D35-42F7-ABEE-9343325C1F32}" name="Nome" dataDxfId="26" totalsRowDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{EFA8F15D-584F-4C04-945A-3DED2B8B5624}" name="Montagem" dataDxfId="24" totalsRowDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7650E1EE-5811-48C9-8355-23A998B379C7}" name="QR Code" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{BB7F2196-2B5F-48C4-9448-0E4DC098762A}" name="Identificador da Montagem  (ID) " dataDxfId="32" totalsRowDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{1C894641-CB47-4458-8D3E-83821726DF13}" name="Peça 1" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{AC6DB513-F3D7-494B-89B0-800144100474}" name="Peça 2" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{5A7909B8-B36B-4D1E-BB35-511363441A82}" name="Peça 3" dataDxfId="26" totalsRowDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{22F8AD07-1F90-4CA5-A0F5-4DA4BFC326EA}" name="Peça 4" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{04291E92-9D35-42F7-ABEE-9343325C1F32}" name="Nome" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{EFA8F15D-584F-4C04-945A-3DED2B8B5624}" name="Montagem" dataDxfId="20" totalsRowDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7650E1EE-5811-48C9-8355-23A998B379C7}" name="QR Code" dataDxfId="18" totalsRowDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAEE89A6-4045-46DA-8B0A-A8F7614937A7}" name="Table_AcademicExpenses64" displayName="Table_AcademicExpenses64" ref="B7:F16" totalsRowShown="0" headerRowDxfId="20" dataDxfId="18" totalsRowDxfId="16" headerRowBorderDxfId="19" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DAEE89A6-4045-46DA-8B0A-A8F7614937A7}" name="Table_AcademicExpenses64" displayName="Table_AcademicExpenses64" ref="B7:F16" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" totalsRowDxfId="11" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="10">
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{74E7D2D3-B442-4085-A649-9E14A2E1EED8}" name="Assembly" dataDxfId="14" totalsRowDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{2B96773D-1149-4682-8095-004001D28840}" name="Step 1" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{5CBFF619-747B-4399-8F8B-3B3FF811D706}" name="Step 2" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{D695FA95-21D4-4BB9-8F20-81669AB91971}" name="Step 3" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{EA9968B6-4B3E-4436-8437-EF6A13BD059D}" name="Step 4" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{74E7D2D3-B442-4085-A649-9E14A2E1EED8}" name="Assembly" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{2B96773D-1149-4682-8095-004001D28840}" name="Step 1" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{5CBFF619-747B-4399-8F8B-3B3FF811D706}" name="Step 2" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{D695FA95-21D4-4BB9-8F20-81669AB91971}" name="Step 3" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{EA9968B6-4B3E-4436-8437-EF6A13BD059D}" name="Step 4" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4411,8 +5098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4431,12 +5118,12 @@
   <sheetData>
     <row r="1" spans="2:13" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:13" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="B2" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="F2" t="s">
         <v>0</v>
       </c>
@@ -4445,7 +5132,7 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="26"/>
     </row>
     <row r="4" spans="2:13" ht="10.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
@@ -4490,10 +5177,10 @@
     </row>
     <row r="8" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="18">
         <v>2</v>
@@ -4510,10 +5197,10 @@
     </row>
     <row r="9" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="18" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <v>2</v>
@@ -4522,7 +5209,7 @@
         <v>2</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="8"/>
@@ -4530,10 +5217,10 @@
     </row>
     <row r="10" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" s="7">
         <v>2</v>
@@ -4542,7 +5229,7 @@
         <v>2</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="8"/>
@@ -4550,10 +5237,10 @@
     </row>
     <row r="11" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="7">
         <v>4</v>
@@ -4562,7 +5249,7 @@
         <v>2</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="8"/>
@@ -4570,10 +5257,10 @@
     </row>
     <row r="12" spans="2:13" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D12" s="18">
         <v>4</v>
@@ -4593,7 +5280,7 @@
     </row>
     <row r="13" spans="2:13" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="18" t="s">
         <v>6</v>
@@ -4682,10 +5369,10 @@
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="28"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
     </row>
     <row r="23" spans="2:16" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
@@ -4733,10 +5420,10 @@
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="25"/>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
     </row>
     <row r="35" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C35" s="1"/>
@@ -4784,12 +5471,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G17:G20">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="62" priority="1">
       <formula>G17&gt;F17</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="61" priority="6">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4840,8 +5527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF356DD-DB4F-4976-BB2F-7A7B3D324CA4}">
   <dimension ref="B1:Q37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="H7" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4861,13 +5548,13 @@
   <sheetData>
     <row r="1" spans="2:17" ht="20" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:17" customFormat="1" ht="95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" t="s">
         <v>0</v>
       </c>
@@ -4931,19 +5618,19 @@
         <v>12345</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" s="18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="8"/>
@@ -4954,20 +5641,20 @@
       <c r="B9" s="18">
         <v>23456</v>
       </c>
-      <c r="C9" s="18">
-        <v>3011</v>
-      </c>
-      <c r="D9" s="18">
-        <v>3437</v>
-      </c>
-      <c r="E9" s="18">
-        <v>76371</v>
-      </c>
-      <c r="F9" s="18">
-        <v>3011</v>
+      <c r="C9" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>27</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="H9"/>
       <c r="I9" s="19"/>
@@ -4980,19 +5667,19 @@
         <v>34567</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="18">
-        <v>3011</v>
-      </c>
-      <c r="E10" s="18">
-        <v>3437</v>
-      </c>
-      <c r="F10" s="18">
-        <v>3011</v>
+        <v>51</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>32</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -5073,11 +5760,11 @@
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="28"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
@@ -5127,11 +5814,11 @@
     </row>
     <row r="30" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
+      <c r="B31" s="27"/>
+      <c r="C31" s="27"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="27"/>
     </row>
     <row r="32" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
@@ -5163,12 +5850,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:H17">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="40" priority="1">
       <formula>H14&gt;G14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:E5">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5219,8 +5906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA1C7DB9-6A79-4D22-A558-4FB1BAC48714}">
   <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="D9" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5240,13 +5927,13 @@
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="2:14" ht="95" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
+      <c r="B2" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
     </row>
     <row r="3" spans="2:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
@@ -5278,19 +5965,19 @@
     </row>
     <row r="7" spans="2:14" s="1" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="F7" s="14" t="s">
         <v>43</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="8" spans="2:14" s="1" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
@@ -5298,39 +5985,61 @@
         <v>12345</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="2:14" s="1" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="18">
+        <v>23456</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>41</v>
-      </c>
-      <c r="F8" s="24" t="s">
+      <c r="E9" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="16"/>
-    </row>
-    <row r="9" spans="2:14" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="2:14" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="7"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
+      <c r="F9" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="16"/>
+    </row>
+    <row r="10" spans="2:14" s="1" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="18">
+        <v>34567</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="2:14" s="10" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="7"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
+      <c r="F11" s="25"/>
     </row>
     <row r="12" spans="2:14" s="3" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="7"/>
@@ -5387,7 +6096,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:E5">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="16" priority="3">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>